<commit_message>
99% added for supply of ridex
</commit_message>
<xml_diff>
--- a/ridex_calc.xlsx
+++ b/ridex_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\toe_contracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EF547C-98FF-4821-8208-8A378EE5306D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B573B3-CABB-45C2-BD9E-1D4BE8B122FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>TOE for add/sub to supply</t>
-  </si>
-  <si>
     <t>TOE 
 (available)</t>
   </si>
@@ -188,6 +185,9 @@
       <t xml:space="preserve">
 1. 1 ride costing around Rs. 5 in the beginning</t>
     </r>
+  </si>
+  <si>
+    <t>TOE for add/sub to supply (99%)</t>
   </si>
 </sst>
 </file>
@@ -607,36 +607,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -661,32 +631,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -698,6 +644,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -707,10 +701,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -750,37 +750,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -848,386 +818,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1651,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1678,7 +1268,7 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -1690,9 +1280,9 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="I2" s="45" t="s">
-        <v>30</v>
+      <c r="E2" s="6"/>
+      <c r="I2" s="43" t="s">
+        <v>29</v>
       </c>
       <c r="J2" s="52"/>
       <c r="K2" s="52"/>
@@ -1702,15 +1292,15 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
       <c r="I3" s="54"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="55"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1722,8 +1312,8 @@
         <v>5</v>
       </c>
       <c r="I4" s="54"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
       <c r="L4" s="55"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1732,29 +1322,29 @@
         <v>1</v>
       </c>
       <c r="I5" s="54"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
       <c r="L5" s="55"/>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I6" s="54"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
       <c r="L6" s="55"/>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
       <c r="I7" s="56"/>
       <c r="J7" s="57"/>
       <c r="K7" s="57"/>
@@ -1771,14 +1361,14 @@
       <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1791,12 +1381,12 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1809,92 +1399,92 @@
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
     </row>
     <row r="13" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="F13" s="43" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="F13" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="42"/>
+      <c r="I13" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="44"/>
-      <c r="I13" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="46"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="45"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="F14" s="39" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="F14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="47"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
       <c r="O14" s="48"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="F15" s="41" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="F15" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="47"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
       <c r="O15" s="48"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
       <c r="O16" s="48"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="49"/>
       <c r="J17" s="50"/>
       <c r="K17" s="50"/>
@@ -1904,70 +1494,70 @@
       <c r="O17" s="51"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:15" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="24" t="s">
+      <c r="F20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1980,37 +1570,37 @@
         <f>SUM(B21)</f>
         <v>-1000</v>
       </c>
-      <c r="D21" s="21">
-        <f>B21*I21</f>
+      <c r="D21" s="11">
+        <f t="shared" ref="D21:D26" si="0">B21*I21</f>
         <v>-999.9990000009999</v>
       </c>
       <c r="E21" s="3">
-        <f>(1/100)*D21</f>
+        <f t="shared" ref="E21:E26" si="1">(1/100)*D21</f>
         <v>-9.9999900000099995</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="11">
         <f>D21-E21</f>
         <v>-989.99901000098987</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="11">
         <v>1000000</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="12">
         <v>1000000</v>
       </c>
-      <c r="I21" s="21">
-        <f>1*G21/(1 + H21)</f>
+      <c r="I21" s="11">
+        <f t="shared" ref="I21:I27" si="2">1*G21/(1 + H21)</f>
         <v>0.99999900000099995</v>
       </c>
-      <c r="J21" s="38">
+      <c r="J21" s="20">
         <f>ABS(E21)</f>
         <v>9.9999900000099995</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -2023,39 +1613,39 @@
         <f>SUM(B21:B22)</f>
         <v>-990</v>
       </c>
-      <c r="D22" s="19">
-        <f>B22*I22</f>
+      <c r="D22" s="9">
+        <f t="shared" si="0"/>
         <v>10.019909880070198</v>
       </c>
       <c r="E22" s="1">
-        <f>(1/100)*D22</f>
+        <f t="shared" si="1"/>
         <v>0.10019909880070199</v>
       </c>
-      <c r="F22" s="19">
-        <f t="shared" ref="F22:F25" si="0">D22-E22</f>
+      <c r="F22" s="9">
+        <f t="shared" ref="F22:F25" si="3">D22-E22</f>
         <v>9.9197107812694956</v>
       </c>
-      <c r="G22" s="19">
-        <f>G21-F21</f>
+      <c r="G22" s="9">
+        <f t="shared" ref="G22:G27" si="4">G21-F21</f>
         <v>1000989.999010001</v>
       </c>
-      <c r="H22" s="20">
-        <f>H21+B21</f>
+      <c r="H22" s="10">
+        <f t="shared" ref="H22:H27" si="5">H21+B21</f>
         <v>999000</v>
       </c>
-      <c r="I22" s="19">
-        <f>1*G22/(1 + H22)</f>
+      <c r="I22" s="9">
+        <f t="shared" si="2"/>
         <v>1.0019909880070199</v>
       </c>
-      <c r="J22" s="37">
-        <f t="shared" ref="J22:J25" si="1">ABS(E22)</f>
+      <c r="J22" s="19">
+        <f t="shared" ref="J22:J25" si="6">ABS(E22)</f>
         <v>0.10019909880070199</v>
       </c>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2068,84 +1658,84 @@
         <f>SUM(B21:B23)</f>
         <v>-1035</v>
       </c>
-      <c r="D23" s="19">
-        <f>B23*I23</f>
+      <c r="D23" s="9">
+        <f t="shared" si="0"/>
         <v>-45.088696289094798</v>
       </c>
       <c r="E23" s="1">
-        <f>(1/100)*D23</f>
+        <f t="shared" si="1"/>
         <v>-0.45088696289094798</v>
       </c>
-      <c r="F23" s="19">
-        <f t="shared" si="0"/>
+      <c r="F23" s="9">
+        <f t="shared" si="3"/>
         <v>-44.63780932620385</v>
       </c>
-      <c r="G23" s="19">
-        <f>G22-F22</f>
+      <c r="G23" s="9">
+        <f t="shared" si="4"/>
         <v>1000980.0792992197</v>
       </c>
-      <c r="H23" s="20">
-        <f>H22+B22</f>
+      <c r="H23" s="10">
+        <f t="shared" si="5"/>
         <v>999010</v>
       </c>
-      <c r="I23" s="19">
-        <f>1*G23/(1 + H23)</f>
+      <c r="I23" s="9">
+        <f t="shared" si="2"/>
         <v>1.0019710286465511</v>
       </c>
-      <c r="J23" s="37">
-        <f t="shared" si="1"/>
+      <c r="J23" s="19">
+        <f t="shared" si="6"/>
         <v>0.45088696289094798</v>
       </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="13">
         <v>200</v>
       </c>
       <c r="C24" s="1">
         <f>SUM(B21:B24)</f>
         <v>-835</v>
       </c>
-      <c r="D24" s="19">
-        <f>B24*I24</f>
+      <c r="D24" s="9">
+        <f t="shared" si="0"/>
         <v>200.41216960508081</v>
       </c>
       <c r="E24" s="1">
-        <f>(1/100)*D24</f>
-        <v>2.0041216960508081</v>
-      </c>
-      <c r="F24" s="19">
-        <f t="shared" si="0"/>
-        <v>198.40804790902999</v>
-      </c>
-      <c r="G24" s="19">
-        <f>G23-F23</f>
-        <v>1001024.7171085458</v>
-      </c>
-      <c r="H24" s="20">
-        <f>H23+B23</f>
-        <v>998965</v>
-      </c>
-      <c r="I24" s="19">
-        <f>1*G24/(1 + H24)</f>
-        <v>1.0020608480254041</v>
-      </c>
-      <c r="J24" s="37">
         <f t="shared" si="1"/>
         <v>2.0041216960508081</v>
       </c>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
+      <c r="F24" s="9">
+        <f t="shared" si="3"/>
+        <v>198.40804790902999</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="4"/>
+        <v>1001024.7171085458</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="5"/>
+        <v>998965</v>
+      </c>
+      <c r="I24" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0020608480254041</v>
+      </c>
+      <c r="J24" s="19">
+        <f t="shared" si="6"/>
+        <v>2.0041216960508081</v>
+      </c>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -2158,39 +1748,39 @@
         <f>SUM(B21:B25)</f>
         <v>-490</v>
       </c>
-      <c r="D25" s="19">
-        <f>B25*I25</f>
+      <c r="D25" s="9">
+        <f t="shared" si="0"/>
         <v>345.57328474539736</v>
       </c>
       <c r="E25" s="1">
-        <f>(1/100)*D25</f>
-        <v>3.4557328474539735</v>
-      </c>
-      <c r="F25" s="19">
-        <f t="shared" si="0"/>
-        <v>342.11755189794337</v>
-      </c>
-      <c r="G25" s="19">
-        <f>G24-F24</f>
-        <v>1000826.3090606368</v>
-      </c>
-      <c r="H25" s="20">
-        <f>H24+B24</f>
-        <v>999165</v>
-      </c>
-      <c r="I25" s="19">
-        <f>1*G25/(1 + H25)</f>
-        <v>1.0016616949141952</v>
-      </c>
-      <c r="J25" s="37">
         <f t="shared" si="1"/>
         <v>3.4557328474539735</v>
       </c>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
+      <c r="F25" s="9">
+        <f t="shared" si="3"/>
+        <v>342.11755189794337</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="4"/>
+        <v>1000826.3090606368</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="5"/>
+        <v>999165</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0016616949141952</v>
+      </c>
+      <c r="J25" s="19">
+        <f t="shared" si="6"/>
+        <v>3.4557328474539735</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -2203,177 +1793,177 @@
         <f>SUM(B21:B26)</f>
         <v>-590</v>
       </c>
-      <c r="D26" s="19">
-        <f>B26*I26</f>
+      <c r="D26" s="9">
+        <f t="shared" si="0"/>
         <v>-100.09736676322109</v>
       </c>
       <c r="E26" s="1">
-        <f>(1/100)*D26</f>
+        <f t="shared" si="1"/>
         <v>-1.000973667632211</v>
       </c>
-      <c r="F26" s="19">
-        <f t="shared" ref="F26" si="2">D26-E26</f>
+      <c r="F26" s="9">
+        <f t="shared" ref="F26" si="7">D26-E26</f>
         <v>-99.09639309558888</v>
       </c>
-      <c r="G26" s="19">
-        <f>G25-F25</f>
+      <c r="G26" s="9">
+        <f t="shared" si="4"/>
         <v>1000484.1915087389</v>
       </c>
-      <c r="H26" s="20">
-        <f>H25+B25</f>
+      <c r="H26" s="10">
+        <f t="shared" si="5"/>
         <v>999510</v>
       </c>
-      <c r="I26" s="19">
-        <f>1*G26/(1 + H26)</f>
+      <c r="I26" s="9">
+        <f t="shared" si="2"/>
         <v>1.000973667632211</v>
       </c>
-      <c r="J26" s="37">
-        <f t="shared" ref="J26" si="3">ABS(E26)</f>
+      <c r="J26" s="19">
+        <f t="shared" ref="J26" si="8">ABS(E26)</f>
         <v>1.000973667632211</v>
       </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="19">
+      <c r="D27" s="9">
         <f>ABS(B27*I27)</f>
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ref="E25:E27" si="4">(0.5/100)*D27</f>
+        <f t="shared" ref="E27" si="9">(0.5/100)*D27</f>
         <v>0</v>
       </c>
-      <c r="F27" s="19">
-        <f t="shared" ref="F27" si="5">D27-E27</f>
+      <c r="F27" s="9">
+        <f t="shared" ref="F27" si="10">D27-E27</f>
         <v>0</v>
       </c>
-      <c r="G27" s="19">
-        <f>G26-F26</f>
+      <c r="G27" s="9">
+        <f t="shared" si="4"/>
         <v>1000583.2879018345</v>
       </c>
-      <c r="H27" s="20">
-        <f>H26+B26</f>
+      <c r="H27" s="10">
+        <f t="shared" si="5"/>
         <v>999410</v>
       </c>
-      <c r="I27" s="19">
-        <f>1*G27/(1 + H27)</f>
+      <c r="I27" s="9">
+        <f t="shared" si="2"/>
         <v>1.0011729787863397</v>
       </c>
-      <c r="J27" s="37">
-        <f t="shared" ref="J27" si="6">ABS(E27)</f>
+      <c r="J27" s="19">
+        <f t="shared" ref="J27" si="11">ABS(E27)</f>
         <v>0</v>
       </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
     </row>
     <row r="33" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
     </row>
     <row r="34" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
     </row>
     <row r="35" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
     </row>
     <row r="36" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2387,51 +1977,51 @@
     <mergeCell ref="I2:L7"/>
   </mergeCells>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"sell"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"sell"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:G14">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"sell"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1 A18:XFD1048576 A13:I13 A14:H17 P13:XFD17 A8:XFD12 A2:I2 A3:H7 M2:XFD7">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"sell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"sell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ridex calc updated: removed calc like multiply 0.99 of expenditure
</commit_message>
<xml_diff>
--- a/ridex_calc.xlsx
+++ b/ridex_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\toe_contracts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D963CED-1014-4A04-BB0F-76D42BD281C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5435833-B8DC-4BC9-8ECD-082FB050F25B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,11 +184,11 @@
     </r>
   </si>
   <si>
-    <t>TOE for add/sub to supply (99%)</t>
-  </si>
-  <si>
     <t>RIDE 
 (available)</t>
+  </si>
+  <si>
+    <t>TOE for add/sub to supply</t>
   </si>
 </sst>
 </file>
@@ -754,6 +754,16 @@
   <dxfs count="12">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -789,16 +799,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1243,7 +1243,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1540,13 +1540,13 @@
         <v>23</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>27</v>
@@ -2019,21 +2019,21 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1 A13:I13 A14:H17 P13:XFD17 A8:XFD12 A2:I2 A3:H7 M2:XFD7 A18:XFD1048576">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"sell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"sell"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>